<commit_message>
test file trailing spaces
</commit_message>
<xml_diff>
--- a/backend/test/resources/bulkUpload/test-excel.xlsx
+++ b/backend/test/resources/bulkUpload/test-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanchan/Projects/gamechanger-web/backend/test/resources/bulkUpload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429DB9DD-1AE4-004A-8C22-CC3E9EAF50B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BEA66C-705E-BB44-AC04-45EDBDA7C332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="500" windowWidth="32000" windowHeight="19060" xr2:uid="{91155129-0587-1B4A-A8D0-D1CB89AEEB30}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Primary Reviewer</t>
   </si>
   <si>
-    <t xml:space="preserve">AI Analysis </t>
-  </si>
-  <si>
     <t>FY22 Label</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>FY22 Service Reviewer</t>
   </si>
   <si>
-    <t xml:space="preserve">Planned Transition Partner </t>
-  </si>
-  <si>
     <t>Current Mission Partners (Academia, Industry, or Other)</t>
   </si>
   <si>
@@ -165,6 +159,12 @@
   </si>
   <si>
     <t>hello it's demo time</t>
+  </si>
+  <si>
+    <t>AI Analysis</t>
+  </si>
+  <si>
+    <t>Planned Transition Partner</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,129 +541,129 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J2">
         <v>2023</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N2">
         <v>3080</v>
       </c>
       <c r="O2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q2">
         <v>4</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S2">
         <v>1</v>
@@ -687,54 +687,54 @@
         <v>981.12199999999996</v>
       </c>
       <c r="AA2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J3">
         <v>2023</v>
       </c>
       <c r="K3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N3">
         <v>3620</v>
       </c>
       <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
         <v>37</v>
-      </c>
-      <c r="P3" t="s">
-        <v>39</v>
       </c>
       <c r="Q3">
         <v>8</v>
       </c>
       <c r="R3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S3">
         <v>2</v>
@@ -761,7 +761,7 @@
         <v>128.79300000000001</v>
       </c>
       <c r="AA3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>